<commit_message>
added a final data table.  Formating and responsive design still to be checked
</commit_message>
<xml_diff>
--- a/data/clinics.xlsx
+++ b/data/clinics.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ba4994e95445f0b/The Code Institute/My Visual Studio Projects/milestone-2-project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunca\OneDrive\The Code Institute\My Visual Studio Projects\milestone-2-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="0473DD55B2028695656D04936637DB4402589DB1" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{7B4AAC18-211F-4C8F-8D5B-5F91D3A7D2A7}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="0473DD55B2028695656D04936637DB4402589DB1" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{E8C16C8A-C5E7-41E4-BDD3-AD0057E65C51}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clinics" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">clinics!$A$1:$Z$62</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="141">
   <si>
     <t>id</t>
   </si>
@@ -407,13 +408,299 @@
   </si>
   <si>
     <t>staff/counsellors</t>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department0; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department1; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department2; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department3; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department4; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department5; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department6; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department7; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department8; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department9; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department10; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.department11; },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) { return d.name; },</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +834,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -890,9 +1188,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1250,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T1" sqref="I1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5526,4 +5827,109 @@
   <autoFilter ref="A1:Z62" xr:uid="{6BB841AD-A325-4F66-8E94-19C2855A0A1E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C62C67-6F25-4746-B6DF-03CF74BC98DB}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>